<commit_message>
added standing cable lateral raise
</commit_message>
<xml_diff>
--- a/dist/exercises.xlsx
+++ b/dist/exercises.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Desktop\Grin and Gain Files\exercise_db_gng\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{52D0261A-5DAB-49CE-ABD0-239F11D273FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6D323-4CA9-4904-95DC-71B59D1025E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB410982-7EC2-4230-AB2C-54975AB6C658}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9487" uniqueCount="3728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9498" uniqueCount="3732">
   <si>
     <t>name</t>
   </si>
@@ -11204,6 +11204,18 @@
   </si>
   <si>
     <t>Nordic_Curls</t>
+  </si>
+  <si>
+    <t>Standing Cable Lateral Raise</t>
+  </si>
+  <si>
+    <t>Standing_Cable_Lateral_Raise</t>
+  </si>
+  <si>
+    <t>["traps", "forearms"]</t>
+  </si>
+  <si>
+    <t>[ "Attach a single-handle to the low pulley cable machine and position it to your left side.", "Stand with your side facing the cable machine and grasp the handle with your right hand, palm facing down, and your left hand resting on your hip.", "Keep a slight bend in your elbow and maintain a neutral spine.", "Exhale as you lift the handle directly to the side, keeping your arm straight but not locked.", "Continue raising the handle until your arm is parallel to the ground or slightly below, ensuring your shoulder is doing the work.", "Pause briefly at the top of the movement, then inhale as you lower the handle back to the starting position in a controlled manner.", "Repeat for the desired number of repetitions, then switch sides and perform the exercise with your left arm." ]</t>
   </si>
 </sst>
 </file>
@@ -11748,8 +11760,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57347AB8-AE8D-4BAF-8AE4-3225684EF00A}" name="Table1" displayName="Table1" ref="A1:K880" totalsRowShown="0">
-  <autoFilter ref="A1:K880" xr:uid="{57347AB8-AE8D-4BAF-8AE4-3225684EF00A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57347AB8-AE8D-4BAF-8AE4-3225684EF00A}" name="Table1" displayName="Table1" ref="A1:K881" totalsRowShown="0">
+  <autoFilter ref="A1:K881" xr:uid="{57347AB8-AE8D-4BAF-8AE4-3225684EF00A}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{480BA1B7-D136-4703-BEB6-580C0A83D0E5}" name="name"/>
     <tableColumn id="3" xr3:uid="{FACC5599-B66A-4623-9D8E-D21DAC1E3C42}" name="force"/>
@@ -12084,10 +12096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398FC8D3-1E6F-4C95-876D-5CC7D8C80D1F}">
-  <dimension ref="A1:K880"/>
+  <dimension ref="A1:K881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A788" workbookViewId="0">
-      <selection activeCell="I870" sqref="I870"/>
+    <sheetView tabSelected="1" topLeftCell="A868" workbookViewId="0">
+      <selection activeCell="G882" sqref="G882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42322,6 +42334,41 @@
         <v>3727</v>
       </c>
     </row>
+    <row r="881" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A881" t="s">
+        <v>3728</v>
+      </c>
+      <c r="B881" t="s">
+        <v>12</v>
+      </c>
+      <c r="C881" t="s">
+        <v>30</v>
+      </c>
+      <c r="D881" t="s">
+        <v>31</v>
+      </c>
+      <c r="E881" t="s">
+        <v>87</v>
+      </c>
+      <c r="F881" t="s">
+        <v>3593</v>
+      </c>
+      <c r="G881" t="s">
+        <v>3730</v>
+      </c>
+      <c r="H881" t="s">
+        <v>3731</v>
+      </c>
+      <c r="I881" t="s">
+        <v>18</v>
+      </c>
+      <c r="J881" t="s">
+        <v>16</v>
+      </c>
+      <c r="K881" t="s">
+        <v>3729</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>